<commit_message>
Criação de pasta para a calculadora
</commit_message>
<xml_diff>
--- a/Documentação/5W2H.xlsx
+++ b/Documentação/5W2H.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/piSPTech/Documentção/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/piSPTech/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{D2348AC7-B968-47CB-80E4-75C1A9732CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECA43868-1C4B-4E92-A057-E5034C5FABD3}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{D2348AC7-B968-47CB-80E4-75C1A9732CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE234E9-4681-4A95-96D8-D5A832D3735F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E69F5D8-D674-44F6-A4BC-9B804A10A670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>PROJETO TI - FERRAMENTA 5W2H</t>
   </si>
@@ -340,12 +340,30 @@
   <si>
     <t>Fabio</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">21/08/2024 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>28/08/2024</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,14 +382,6 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,9 +441,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -806,8 +813,8 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,15 +828,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -850,7 +857,7 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -873,7 +880,7 @@
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -963,8 +970,8 @@
       <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>39</v>
+      <c r="G7" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1003,7 +1010,9 @@
       <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1021,8 +1030,12 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1040,8 +1053,12 @@
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1059,8 +1076,12 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>56</v>
       </c>
@@ -1078,8 +1099,12 @@
       <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Atualização da planilha 5W2H
</commit_message>
<xml_diff>
--- a/Documentação/5W2H.xlsx
+++ b/Documentação/5W2H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/piSPTech/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{D2348AC7-B968-47CB-80E4-75C1A9732CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE234E9-4681-4A95-96D8-D5A832D3735F}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="8_{D2348AC7-B968-47CB-80E4-75C1A9732CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C574FF-FC07-46F9-8047-1A8BDF0F596C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E69F5D8-D674-44F6-A4BC-9B804A10A670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>PROJETO TI - FERRAMENTA 5W2H</t>
   </si>
@@ -221,21 +221,6 @@
     <t>Entregável PI e BD</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">30/08/2024 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06/09/2024</t>
-    </r>
-  </si>
-  <si>
     <t>Plataforma MySQL</t>
   </si>
   <si>
@@ -356,6 +341,51 @@
         <scheme val="minor"/>
       </rPr>
       <t>28/08/2024</t>
+    </r>
+  </si>
+  <si>
+    <t>Apresentação em PowerPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação para o cliente </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">05/09/2024 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12/09/2024</t>
+    </r>
+  </si>
+  <si>
+    <t>PowerPoint</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução de Negócio</t>
+  </si>
+  <si>
+    <t>Canva, Diagrams ou PowerPoint</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30/08/2024 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12/09/2024</t>
     </r>
   </si>
 </sst>
@@ -394,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,13 +433,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF3FFF3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFEFFD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,12 +468,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -440,20 +479,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -478,6 +564,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFFEFFD5"/>
+      <color rgb="FFF3FFF3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -487,10 +580,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,452 +899,504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1B3561-074C-4BD3-BE9B-D71B1F81068B}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="11" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="G17" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="G2:G3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G15">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Em execução">
+  <conditionalFormatting sqref="G4:G17">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Em execução">
       <formula>NOT(ISERROR(SEARCH("Em execução",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Não iniciado">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Não iniciado">
       <formula>NOT(ISERROR(SEARCH("Não iniciado",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G15" xr:uid="{D2021284-5622-4585-B194-69B9A4B5045B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G17" xr:uid="{D2021284-5622-4585-B194-69B9A4B5045B}">
       <formula1>"OK, Em execução, Não iniciado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>